<commit_message>
New Pedal Control Plugin
</commit_message>
<xml_diff>
--- a/Docs/Race Engineer Rule Memory Structure.xlsx
+++ b/Docs/Race Engineer Rule Memory Structure.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Controller\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CCD18E36-E3BA-4815-8761-CE70787CA2A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC17952-7724-42FD-8885-E5AA6A6F7598}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="2985" windowWidth="21945" windowHeight="10305"/>
+    <workbookView xWindow="1200" yWindow="2595" windowWidth="21945" windowHeight="10305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Race Engineer Rule Memory Struc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="70">
   <si>
     <t>Race</t>
   </si>
@@ -64,9 +64,6 @@
     <t>See Damage.Repair</t>
   </si>
   <si>
-    <t>[Integer] (PSI * 10)</t>
-  </si>
-  <si>
     <t>Weather</t>
   </si>
   <si>
@@ -214,25 +211,31 @@
     <t>[Integer] (Time of Lap Start in MilliSeconds)</t>
   </si>
   <si>
-    <t>[Integer]  (Unit 1000 Gram)</t>
-  </si>
-  <si>
     <t>Pressure</t>
   </si>
   <si>
     <t>Temperature</t>
   </si>
   <si>
-    <t>Pressures</t>
-  </si>
-  <si>
     <t>[Float] (Degrees Celsius)</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>[Float]</t>
+  </si>
+  <si>
+    <t>AvgConsumption</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1066,573 +1069,622 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>57</v>
       </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>55</v>
       </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>49</v>
+      </c>
+      <c r="G38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" t="s">
+        <v>29</v>
+      </c>
+      <c r="G41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="D44" t="s">
+        <v>39</v>
+      </c>
+      <c r="E44" t="s">
+        <v>42</v>
+      </c>
+      <c r="G44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>43</v>
+      </c>
+      <c r="G45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>44</v>
+      </c>
+      <c r="G46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>46</v>
+      </c>
+      <c r="G48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" t="s">
+        <v>48</v>
+      </c>
+      <c r="G49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>49</v>
+      </c>
+      <c r="G50" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>50</v>
+      </c>
+      <c r="G51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>51</v>
+      </c>
+      <c r="G52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" t="s">
+        <v>6</v>
+      </c>
+      <c r="H55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>36</v>
+      </c>
+      <c r="G58" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>63</v>
+      </c>
+      <c r="E59" t="s">
+        <v>48</v>
+      </c>
+      <c r="G59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>49</v>
+      </c>
+      <c r="G60" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>50</v>
+      </c>
+      <c r="G61" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>51</v>
+      </c>
+      <c r="G62" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="D63" t="s">
+        <v>29</v>
+      </c>
+      <c r="G63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>30</v>
+      </c>
+      <c r="G64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" t="s">
+        <v>38</v>
+      </c>
+      <c r="G65" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>39</v>
+      </c>
+      <c r="G66" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>20</v>
       </c>
-      <c r="F19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" t="s">
-        <v>49</v>
-      </c>
-      <c r="F27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E29" t="s">
-        <v>51</v>
-      </c>
-      <c r="F29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" t="s">
-        <v>49</v>
-      </c>
-      <c r="F31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
-        <v>51</v>
-      </c>
-      <c r="F33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35" t="s">
-        <v>30</v>
-      </c>
-      <c r="F35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="G68" t="s">
+        <v>6</v>
+      </c>
+      <c r="H68" t="s">
         <v>40</v>
-      </c>
-      <c r="E38" t="s">
-        <v>43</v>
-      </c>
-      <c r="F38" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E39" t="s">
-        <v>44</v>
-      </c>
-      <c r="F39" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
-        <v>45</v>
-      </c>
-      <c r="F40" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E41" t="s">
-        <v>46</v>
-      </c>
-      <c r="F41" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" t="s">
-        <v>39</v>
-      </c>
-      <c r="E43" t="s">
-        <v>49</v>
-      </c>
-      <c r="F43" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E44" t="s">
-        <v>50</v>
-      </c>
-      <c r="F44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E45" t="s">
-        <v>51</v>
-      </c>
-      <c r="F45" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E46" t="s">
-        <v>52</v>
-      </c>
-      <c r="F46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>21</v>
-      </c>
-      <c r="F48" t="s">
-        <v>6</v>
-      </c>
-      <c r="G48" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>23</v>
-      </c>
-      <c r="F49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G49" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>25</v>
-      </c>
-      <c r="F50" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>28</v>
-      </c>
-      <c r="D51" t="s">
-        <v>36</v>
-      </c>
-      <c r="F51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
-        <v>37</v>
-      </c>
-      <c r="F52" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
-        <v>65</v>
-      </c>
-      <c r="E53" t="s">
-        <v>49</v>
-      </c>
-      <c r="F53" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E54" t="s">
-        <v>50</v>
-      </c>
-      <c r="F54" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E55" t="s">
-        <v>51</v>
-      </c>
-      <c r="F55" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E56" t="s">
-        <v>52</v>
-      </c>
-      <c r="F56" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>29</v>
-      </c>
-      <c r="D57" t="s">
-        <v>30</v>
-      </c>
-      <c r="F57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
-        <v>31</v>
-      </c>
-      <c r="F58" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
-        <v>9</v>
-      </c>
-      <c r="D59" t="s">
-        <v>39</v>
-      </c>
-      <c r="F59" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>40</v>
-      </c>
-      <c r="F60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>21</v>
-      </c>
-      <c r="F62" t="s">
-        <v>6</v>
-      </c>
-      <c r="G62" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AI Race Engineer Part 2
</commit_message>
<xml_diff>
--- a/Docs/Race Engineer Rule Memory Structure.xlsx
+++ b/Docs/Race Engineer Rule Memory Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Controller\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC17952-7724-42FD-8885-E5AA6A6F7598}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5334B036-BB3A-4E2C-A257-2273CDE6D175}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="2595" windowWidth="21945" windowHeight="10305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="72">
   <si>
     <t>Race</t>
   </si>
@@ -37,15 +37,9 @@
     <t>InLap</t>
   </si>
   <si>
-    <t>[Integer] (Lap Time in Seconds)</t>
-  </si>
-  <si>
     <t>[Integer]</t>
   </si>
   <si>
-    <t>First fresh tyre set, when race starts</t>
-  </si>
-  <si>
     <t>Damage</t>
   </si>
   <si>
@@ -187,15 +181,9 @@
     <t>AvgLapTime</t>
   </si>
   <si>
-    <t>FreshTyreSet</t>
-  </si>
-  <si>
     <t>Car</t>
   </si>
   <si>
-    <t>Tracke</t>
-  </si>
-  <si>
     <t>[Integer] (Race Duration in Seconds)</t>
   </si>
   <si>
@@ -230,6 +218,24 @@
   </si>
   <si>
     <t>AvgConsumption</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>#NR# of the last pitstop</t>
+  </si>
+  <si>
+    <t>Tyre set, when race starts</t>
+  </si>
+  <si>
+    <t>Fresh</t>
+  </si>
+  <si>
+    <t>First fresh tyre set</t>
+  </si>
+  <si>
+    <t>[Integer] (Lap Time in Milliseconds)</t>
   </si>
 </sst>
 </file>
@@ -1070,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,18 +1096,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1109,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1130,287 +1136,293 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>55</v>
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
       </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
         <v>63</v>
       </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>49</v>
-      </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>67</v>
-      </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" t="s">
         <v>51</v>
       </c>
-      <c r="G19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>20</v>
       </c>
-      <c r="B26" t="s">
+      <c r="G29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
         <v>21</v>
       </c>
-      <c r="C26" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
-        <v>60</v>
-      </c>
-      <c r="G29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" t="s">
-        <v>25</v>
-      </c>
       <c r="G30" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="G31" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="G32" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>27</v>
-      </c>
       <c r="D33" t="s">
-        <v>63</v>
-      </c>
-      <c r="E33" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="G33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
-        <v>49</v>
+      <c r="D34" t="s">
+        <v>65</v>
       </c>
       <c r="G34" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" t="s">
+        <v>59</v>
+      </c>
       <c r="E35" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G35" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G36" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>64</v>
-      </c>
       <c r="E37" t="s">
         <v>48</v>
       </c>
       <c r="G37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
@@ -1418,273 +1430,306 @@
         <v>49</v>
       </c>
       <c r="G38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>60</v>
+      </c>
       <c r="E39" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G39" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G40" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" t="s">
-        <v>29</v>
+      <c r="E41" t="s">
+        <v>48</v>
       </c>
       <c r="G41" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
-        <v>30</v>
+      <c r="E42" t="s">
+        <v>49</v>
       </c>
       <c r="G42" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>14</v>
+        <v>60</v>
+      </c>
+      <c r="D43" t="s">
+        <v>27</v>
       </c>
       <c r="G43" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>8</v>
-      </c>
       <c r="D44" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" t="s">
         <v>39</v>
       </c>
-      <c r="E44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G44" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E45" t="s">
-        <v>43</v>
-      </c>
-      <c r="G45" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>37</v>
+      </c>
       <c r="E46" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G46" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
+        <v>41</v>
+      </c>
+      <c r="G47" t="s">
         <v>45</v>
-      </c>
-      <c r="G47" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" t="s">
-        <v>38</v>
-      </c>
       <c r="E49" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G50" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>36</v>
+      </c>
       <c r="E51" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G51" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G52" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>48</v>
+      </c>
+      <c r="G53" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>31</v>
-      </c>
-      <c r="B54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C54" t="s">
-        <v>20</v>
+      <c r="E54" t="s">
+        <v>49</v>
       </c>
       <c r="G54" t="s">
-        <v>6</v>
-      </c>
-      <c r="H54" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>22</v>
-      </c>
-      <c r="G55" t="s">
-        <v>6</v>
-      </c>
-      <c r="H55" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" t="s">
+        <v>19</v>
+      </c>
       <c r="C56" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G56" t="s">
-        <v>34</v>
+        <v>5</v>
+      </c>
+      <c r="H56" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>27</v>
-      </c>
-      <c r="D57" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57" t="s">
+        <v>5</v>
+      </c>
+      <c r="H57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" t="s">
+        <v>33</v>
+      </c>
+      <c r="G59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>34</v>
+      </c>
+      <c r="G60" t="s">
         <v>35</v>
       </c>
-      <c r="G57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
-        <v>36</v>
-      </c>
-      <c r="G58" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
-        <v>63</v>
-      </c>
-      <c r="E59" t="s">
-        <v>48</v>
-      </c>
-      <c r="G59" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E60" t="s">
-        <v>49</v>
-      </c>
-      <c r="G60" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>59</v>
+      </c>
       <c r="E61" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G61" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G62" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
-        <v>28</v>
-      </c>
-      <c r="D63" t="s">
-        <v>29</v>
+      <c r="E63" t="s">
+        <v>48</v>
       </c>
       <c r="G63" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D64" t="s">
-        <v>30</v>
+      <c r="E64" t="s">
+        <v>49</v>
       </c>
       <c r="G64" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D65" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="G65" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>36</v>
+      </c>
+      <c r="G67" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>20</v>
+      <c r="D68" t="s">
+        <v>37</v>
       </c>
       <c r="G68" t="s">
-        <v>6</v>
-      </c>
-      <c r="H68" t="s">
-        <v>40</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70" t="s">
+        <v>66</v>
+      </c>
+      <c r="G70" t="s">
+        <v>5</v>
+      </c>
+      <c r="H70" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72" t="s">
+        <v>5</v>
+      </c>
+      <c r="H72" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AI Race Engineer Part 3
</commit_message>
<xml_diff>
--- a/Docs/Race Engineer Rule Memory Structure.xlsx
+++ b/Docs/Race Engineer Rule Memory Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Controller\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5334B036-BB3A-4E2C-A257-2273CDE6D175}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514BF57F-9BA4-4EDF-B9E7-AAEBC83BBF0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="2595" windowWidth="21945" windowHeight="10305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="82">
   <si>
     <t>Race</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Repair</t>
   </si>
   <si>
-    <t>[1=Always; 2=Impact; 3=Above Threshold]</t>
-  </si>
-  <si>
     <t>Threshold</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>Tyre</t>
   </si>
   <si>
-    <t>Temp</t>
-  </si>
-  <si>
     <t>Air</t>
   </si>
   <si>
@@ -112,12 +106,6 @@
     <t>Pitstop</t>
   </si>
   <si>
-    <t>#Nr# will be "PLANNED" and Lap might be missing for the next pitstop</t>
-  </si>
-  <si>
-    <t>Actual time for concluded, and estimated time for planned pitstops</t>
-  </si>
-  <si>
     <t>[Integer] (Unit 1000 Gram)</t>
   </si>
   <si>
@@ -178,18 +166,12 @@
     <t>[String]</t>
   </si>
   <si>
-    <t>AvgLapTime</t>
-  </si>
-  <si>
     <t>Car</t>
   </si>
   <si>
     <t>[Integer] (Race Duration in Seconds)</t>
   </si>
   <si>
-    <t>AvgFuelPerLap</t>
-  </si>
-  <si>
     <t>End</t>
   </si>
   <si>
@@ -236,6 +218,54 @@
   </si>
   <si>
     <t>[Integer] (Lap Time in Milliseconds)</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>AvgTime</t>
+  </si>
+  <si>
+    <t>Deviation</t>
+  </si>
+  <si>
+    <t>Allowed deviation from target pressure, before a pressure change will be triggered</t>
+  </si>
+  <si>
+    <t>Considered</t>
+  </si>
+  <si>
+    <t>The number of laps before the current one, which are considered for the statistical calculations</t>
+  </si>
+  <si>
+    <t>Tyre compound, when race starts</t>
+  </si>
+  <si>
+    <t>Tyre pressure, when race starts</t>
+  </si>
+  <si>
+    <t>Dry</t>
+  </si>
+  <si>
+    <t>Pressure target for warm dry tyres</t>
+  </si>
+  <si>
+    <t>Wet</t>
+  </si>
+  <si>
+    <t>End of lap time, where the pitstop has been performed</t>
+  </si>
+  <si>
+    <t>[1=Always; 2=Impact; 3=Threshold]</t>
+  </si>
+  <si>
+    <t>[Float] (Unit 1000 Gram)</t>
+  </si>
+  <si>
+    <t>SafetyMargin</t>
+  </si>
+  <si>
+    <t>[0=Never;1=Always; 2=Impact; 3=Threshold]</t>
   </si>
 </sst>
 </file>
@@ -1076,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,649 +1117,788 @@
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="63.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" t="s">
+        <v>58</v>
+      </c>
+      <c r="I26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" t="s">
+        <v>58</v>
+      </c>
+      <c r="I27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" t="s">
+        <v>58</v>
+      </c>
+      <c r="I28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="H36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>50</v>
+      </c>
+      <c r="H39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>59</v>
+      </c>
+      <c r="H42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" t="s">
+        <v>42</v>
+      </c>
+      <c r="H43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>43</v>
+      </c>
+      <c r="H44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>44</v>
+      </c>
+      <c r="H45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>45</v>
+      </c>
+      <c r="H46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="E47" t="s">
+        <v>42</v>
+      </c>
+      <c r="H47" t="s">
         <v>55</v>
       </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>56</v>
-      </c>
-      <c r="G31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>24</v>
-      </c>
-      <c r="G33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>65</v>
-      </c>
-      <c r="G34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" t="s">
-        <v>59</v>
-      </c>
-      <c r="E35" t="s">
-        <v>46</v>
-      </c>
-      <c r="G35" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E36" t="s">
-        <v>47</v>
-      </c>
-      <c r="G36" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E37" t="s">
-        <v>48</v>
-      </c>
-      <c r="G37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E38" t="s">
-        <v>49</v>
-      </c>
-      <c r="G38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39" t="s">
-        <v>46</v>
-      </c>
-      <c r="G39" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
-        <v>47</v>
-      </c>
-      <c r="G40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E41" t="s">
-        <v>48</v>
-      </c>
-      <c r="G41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E42" t="s">
-        <v>49</v>
-      </c>
-      <c r="G42" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" t="s">
-        <v>27</v>
-      </c>
-      <c r="G43" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>28</v>
-      </c>
-      <c r="G44" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" t="s">
-        <v>37</v>
-      </c>
-      <c r="E46" t="s">
-        <v>40</v>
-      </c>
-      <c r="G46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E47" t="s">
-        <v>41</v>
-      </c>
-      <c r="G47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
-        <v>42</v>
-      </c>
-      <c r="G48" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="H48" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
-        <v>43</v>
-      </c>
-      <c r="G49" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="H49" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
-        <v>44</v>
-      </c>
-      <c r="G50" t="s">
         <v>45</v>
+      </c>
+      <c r="H50" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" t="s">
+        <v>25</v>
+      </c>
+      <c r="H51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>26</v>
+      </c>
+      <c r="H52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
         <v>6</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D54" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" t="s">
         <v>36</v>
       </c>
-      <c r="E51" t="s">
-        <v>46</v>
-      </c>
-      <c r="G51" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E52" t="s">
-        <v>47</v>
-      </c>
-      <c r="G52" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E53" t="s">
-        <v>48</v>
-      </c>
-      <c r="G53" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E54" t="s">
-        <v>49</v>
-      </c>
-      <c r="G54" t="s">
-        <v>45</v>
+      <c r="H54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>37</v>
+      </c>
+      <c r="H55" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>29</v>
-      </c>
-      <c r="B56" t="s">
-        <v>19</v>
-      </c>
-      <c r="C56" t="s">
-        <v>18</v>
-      </c>
-      <c r="G56" t="s">
-        <v>5</v>
+      <c r="E56" t="s">
+        <v>38</v>
       </c>
       <c r="H56" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>20</v>
-      </c>
-      <c r="G57" t="s">
-        <v>5</v>
+      <c r="E57" t="s">
+        <v>39</v>
       </c>
       <c r="H57" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>22</v>
-      </c>
-      <c r="G58" t="s">
-        <v>32</v>
+      <c r="E58" t="s">
+        <v>40</v>
+      </c>
+      <c r="H58" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>33</v>
-      </c>
-      <c r="G59" t="s">
-        <v>5</v>
+        <v>32</v>
+      </c>
+      <c r="E59" t="s">
+        <v>42</v>
+      </c>
+      <c r="H59" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>34</v>
-      </c>
-      <c r="G60" t="s">
-        <v>35</v>
+      <c r="E60" t="s">
+        <v>43</v>
+      </c>
+      <c r="H60" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>59</v>
-      </c>
       <c r="E61" t="s">
-        <v>46</v>
-      </c>
-      <c r="G61" t="s">
-        <v>64</v>
+        <v>44</v>
+      </c>
+      <c r="H61" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
-        <v>47</v>
-      </c>
-      <c r="G62" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E63" t="s">
-        <v>48</v>
-      </c>
-      <c r="G63" t="s">
-        <v>64</v>
+        <v>45</v>
+      </c>
+      <c r="H62" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E64" t="s">
-        <v>49</v>
-      </c>
-      <c r="G64" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" t="s">
+        <v>17</v>
+      </c>
+      <c r="H64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" t="s">
+        <v>5</v>
+      </c>
+      <c r="I65" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>21</v>
+      </c>
+      <c r="H66" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67" t="s">
+        <v>29</v>
+      </c>
+      <c r="H67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>30</v>
+      </c>
+      <c r="H68" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>53</v>
+      </c>
+      <c r="E69" t="s">
+        <v>42</v>
+      </c>
+      <c r="H69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
+        <v>43</v>
+      </c>
+      <c r="H70" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>44</v>
+      </c>
+      <c r="H71" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>45</v>
+      </c>
+      <c r="H72" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>54</v>
+      </c>
+      <c r="D73" t="s">
+        <v>25</v>
+      </c>
+      <c r="H73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
         <v>26</v>
       </c>
-      <c r="D65" t="s">
+      <c r="H74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" t="s">
+        <v>32</v>
+      </c>
+      <c r="H75" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>33</v>
+      </c>
+      <c r="H76" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>27</v>
       </c>
-      <c r="G65" t="s">
+      <c r="B78" t="s">
+        <v>60</v>
+      </c>
+      <c r="H78" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D66" t="s">
-        <v>28</v>
-      </c>
-      <c r="G66" t="s">
+      <c r="I78" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>17</v>
+      </c>
+      <c r="H80" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
-        <v>7</v>
-      </c>
-      <c r="D67" t="s">
-        <v>36</v>
-      </c>
-      <c r="G67" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
-        <v>37</v>
-      </c>
-      <c r="G68" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>29</v>
-      </c>
-      <c r="B70" t="s">
-        <v>66</v>
-      </c>
-      <c r="G70" t="s">
-        <v>5</v>
-      </c>
-      <c r="H70" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>18</v>
-      </c>
-      <c r="G72" t="s">
-        <v>5</v>
-      </c>
-      <c r="H72" t="s">
-        <v>38</v>
+      <c r="I80" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AI Race Engineer Part 4
</commit_message>
<xml_diff>
--- a/Docs/Race Engineer Rule Memory Structure.xlsx
+++ b/Docs/Race Engineer Rule Memory Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Controller\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514BF57F-9BA4-4EDF-B9E7-AAEBC83BBF0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C213FD6F-361A-4B27-833B-5B1AA002AB49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="2595" windowWidth="21945" windowHeight="10305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="85">
   <si>
     <t>Race</t>
   </si>
@@ -266,6 +266,15 @@
   </si>
   <si>
     <t>[0=Never;1=Always; 2=Impact; 3=Threshold]</t>
+  </si>
+  <si>
+    <t>[integer]</t>
+  </si>
+  <si>
+    <t>Number of remaing laps, when the race engineer will warn for an upcoming pitstop</t>
+  </si>
+  <si>
+    <t>PitstopWarning</t>
   </si>
 </sst>
 </file>
@@ -1106,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,9 +1188,6 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
       <c r="D7" t="s">
         <v>80</v>
       </c>
@@ -1190,14 +1196,14 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>82</v>
+      </c>
+      <c r="I8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,105 +1211,105 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
         <v>70</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>5</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>7</v>
       </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
       <c r="H11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
       <c r="E13" t="s">
         <v>7</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
         <v>8</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" t="s">
         <v>9</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>74</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>53</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>56</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>42</v>
       </c>
-      <c r="H14" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H16" t="s">
         <v>58</v>
@@ -1311,46 +1317,46 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
         <v>45</v>
       </c>
-      <c r="H17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>24</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>76</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>53</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>56</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>42</v>
       </c>
-      <c r="H18" t="s">
-        <v>58</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="H19" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H19" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H20" t="s">
         <v>58</v>
@@ -1358,82 +1364,79 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
         <v>45</v>
       </c>
-      <c r="H21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
+      <c r="H22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
         <v>68</v>
       </c>
-      <c r="H22" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="H23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
         <v>29</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>63</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H24" t="s">
         <v>5</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>24</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>30</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H25" t="s">
         <v>31</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I25" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>29</v>
-      </c>
-      <c r="H25" t="s">
-        <v>5</v>
-      </c>
-      <c r="I25" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
         <v>53</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>42</v>
-      </c>
-      <c r="H26" t="s">
-        <v>58</v>
-      </c>
-      <c r="I26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E27" t="s">
-        <v>43</v>
       </c>
       <c r="H27" t="s">
         <v>58</v>
@@ -1444,7 +1447,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H28" t="s">
         <v>58</v>
@@ -1455,7 +1458,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H29" t="s">
         <v>58</v>
@@ -1464,31 +1467,34 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" t="s">
+        <v>58</v>
+      </c>
+      <c r="I30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>11</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>12</v>
-      </c>
-      <c r="H31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" t="s">
-        <v>14</v>
       </c>
       <c r="H32" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H33" t="s">
         <v>35</v>
@@ -1496,64 +1502,64 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H34" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>17</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>18</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>46</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H37" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>19</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H39" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+      <c r="D40" t="s">
+        <v>50</v>
+      </c>
+      <c r="H40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>21</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>22</v>
-      </c>
-      <c r="H40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
-        <v>23</v>
       </c>
       <c r="H41" t="s">
         <v>58</v>
@@ -1561,29 +1567,29 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
         <v>59</v>
       </c>
-      <c r="H42" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+      <c r="H43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>24</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>53</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>42</v>
-      </c>
-      <c r="H43" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E44" t="s">
-        <v>43</v>
       </c>
       <c r="H44" t="s">
         <v>58</v>
@@ -1591,7 +1597,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H45" t="s">
         <v>58</v>
@@ -1599,224 +1605,224 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
+        <v>44</v>
+      </c>
+      <c r="H46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
         <v>45</v>
       </c>
-      <c r="H46" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
+      <c r="H47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
         <v>54</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>42</v>
-      </c>
-      <c r="H47" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E48" t="s">
-        <v>43</v>
       </c>
       <c r="H48" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H49" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H50" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>54</v>
-      </c>
-      <c r="D51" t="s">
-        <v>25</v>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>45</v>
       </c>
       <c r="H51" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>54</v>
+      </c>
       <c r="D52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H52" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>26</v>
+      </c>
+      <c r="H53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
         <v>11</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H54" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
         <v>6</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>33</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E55" t="s">
         <v>36</v>
-      </c>
-      <c r="H54" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E55" t="s">
-        <v>37</v>
       </c>
       <c r="H55" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H56" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H57" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H58" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" t="s">
-        <v>32</v>
-      </c>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H59" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>32</v>
+      </c>
       <c r="E60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H60" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H61" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H62" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>45</v>
+      </c>
+      <c r="H63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>27</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>18</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>17</v>
-      </c>
-      <c r="H64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
-        <v>19</v>
       </c>
       <c r="H65" t="s">
         <v>5</v>
       </c>
-      <c r="I65" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H66" t="s">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="I66" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
+        <v>21</v>
+      </c>
+      <c r="H67" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
         <v>24</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>29</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H68" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
-        <v>30</v>
-      </c>
-      <c r="H68" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
+        <v>30</v>
+      </c>
+      <c r="H69" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
         <v>53</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E70" t="s">
         <v>42</v>
-      </c>
-      <c r="H69" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E70" t="s">
-        <v>43</v>
       </c>
       <c r="H70" t="s">
         <v>58</v>
@@ -1824,7 +1830,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H71" t="s">
         <v>58</v>
@@ -1832,72 +1838,80 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
+        <v>44</v>
+      </c>
+      <c r="H72" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
         <v>45</v>
       </c>
-      <c r="H72" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
+      <c r="H73" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
         <v>54</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D74" t="s">
         <v>25</v>
-      </c>
-      <c r="H73" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
-        <v>26</v>
       </c>
       <c r="H74" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
+      <c r="D75" t="s">
+        <v>26</v>
+      </c>
+      <c r="H75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
         <v>7</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>32</v>
-      </c>
-      <c r="H75" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
-        <v>33</v>
       </c>
       <c r="H76" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>33</v>
+      </c>
+      <c r="H77" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>27</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>60</v>
       </c>
-      <c r="H78" t="s">
+      <c r="H79" t="s">
         <v>5</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I79" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>17</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H81" t="s">
         <v>5</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I81" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>